<commit_message>
5 strun ladi dobre. hluboke maj problem
</commit_message>
<xml_diff>
--- a/ADC DATA/pll parametry.xlsx
+++ b/ADC DATA/pll parametry.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\H116261\Documents\GitHub\AutotuneGuitar\ADC DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITfiles\AutotuneGuitar\ADC DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000000"/>
   </numFmts>
@@ -94,7 +94,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -408,14 +408,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.25">
@@ -558,10 +559,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +570,7 @@
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -577,73 +578,103 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2">
         <f>C1*POWER(2,1/12)</f>
         <v>1.0594630943592953</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>440</v>
+      </c>
+      <c r="J2">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C15" si="0">C2*POWER(2,1/12)</f>
+        <f t="shared" ref="C3:C13" si="0">C2*POWER(2,1/12)</f>
         <v>1.122462048309373</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f>1/I2</f>
+        <v>2.2727272727272726E-3</v>
+      </c>
+      <c r="J3">
+        <f>1/J2</f>
+        <v>2.5000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="2">
         <f t="shared" si="0"/>
         <v>1.1892071150027212</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>1.2599210498948734</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>1.3348398541700346</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f>I3/J3</f>
+        <v>909.09090909090901</v>
+      </c>
+      <c r="J6">
+        <f>I6*4</f>
+        <v>3636.363636363636</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>1.4142135623730954</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f>I6*$C6</f>
+        <v>1213.4907765182131</v>
+      </c>
+      <c r="J7">
+        <f>J6*$C6</f>
+        <v>4853.9631060728525</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>1.498307076876682</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f>C8*POWER(2,1/12)</f>
         <v>1.5874010519682</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>1.6817928305074297</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>1.7817974362806792</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>1.8877486253633877</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13">
         <f t="shared" si="0"/>
         <v>2.0000000000000009</v>

</xml_diff>